<commit_message>
Add Fresno State roster and fix error in Stanford roster
</commit_message>
<xml_diff>
--- a/data/datasets/roster_stanford.xlsx
+++ b/data/datasets/roster_stanford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE34A6-E785-4A3B-92D3-788586362577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E52150-3A79-4432-9522-F916BC7C8BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7338,8 +7338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8596,7 +8596,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>97</v>
@@ -8631,7 +8631,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Fix position and group for Tevita Law row of 2029 stanford roster
</commit_message>
<xml_diff>
--- a/data/datasets/roster_stanford.xlsx
+++ b/data/datasets/roster_stanford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166FC7FC-1AE7-4F9A-896E-96017F13883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8958708-633A-4621-A0AD-D2FB516A0000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7567,8 +7567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9424,10 +9424,10 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Create 2029 roster charts
</commit_message>
<xml_diff>
--- a/data/datasets/roster_stanford.xlsx
+++ b/data/datasets/roster_stanford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE597A1-AB20-42E1-9C2C-F6AB95A72968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B376987B-5869-44A6-9327-5221DD619CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1160,7 +1160,13 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Frame2" displayName="Frame2" ref="A1:L86" totalsRowShown="0">
-  <autoFilter ref="A1:L86" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <autoFilter ref="A1:L86" xr:uid="{00000000-0009-0000-0100-000003000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="WR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="first_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="last_name"/>
@@ -7573,7 +7579,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7629,7 +7637,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -7664,7 +7672,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -7699,7 +7707,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>218</v>
       </c>
@@ -7734,7 +7742,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -7769,7 +7777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -7804,7 +7812,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -7839,7 +7847,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>284</v>
       </c>
@@ -7874,7 +7882,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>286</v>
       </c>
@@ -7909,7 +7917,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>288</v>
       </c>
@@ -8224,7 +8232,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>336</v>
       </c>
@@ -8259,7 +8267,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>249</v>
       </c>
@@ -8294,7 +8302,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>297</v>
       </c>
@@ -8329,7 +8337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>299</v>
       </c>
@@ -8364,7 +8372,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -8399,7 +8407,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>111</v>
       </c>
@@ -8434,7 +8442,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>255</v>
       </c>
@@ -8469,7 +8477,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
@@ -8504,7 +8512,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -8539,7 +8547,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>97</v>
       </c>
@@ -8574,7 +8582,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>99</v>
       </c>
@@ -8609,7 +8617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>114</v>
       </c>
@@ -8644,7 +8652,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>303</v>
       </c>
@@ -8679,7 +8687,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
@@ -8714,7 +8722,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
@@ -8749,7 +8757,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>115</v>
       </c>
@@ -8784,7 +8792,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
@@ -8819,7 +8827,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>202</v>
       </c>
@@ -8854,7 +8862,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
@@ -8889,7 +8897,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>119</v>
       </c>
@@ -8924,7 +8932,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>305</v>
       </c>
@@ -8959,7 +8967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>157</v>
       </c>
@@ -8994,7 +9002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>164</v>
       </c>
@@ -9029,7 +9037,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>257</v>
       </c>
@@ -9064,7 +9072,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>259</v>
       </c>
@@ -9099,7 +9107,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>315</v>
       </c>
@@ -9134,7 +9142,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
@@ -9169,7 +9177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>140</v>
       </c>
@@ -9204,7 +9212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>309</v>
       </c>
@@ -9239,7 +9247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>311</v>
       </c>
@@ -9274,7 +9282,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>313</v>
       </c>
@@ -9309,7 +9317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>128</v>
       </c>
@@ -9344,7 +9352,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
@@ -9379,7 +9387,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>144</v>
       </c>
@@ -9414,7 +9422,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>261</v>
       </c>
@@ -9449,7 +9457,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>265</v>
       </c>
@@ -9484,7 +9492,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>159</v>
       </c>
@@ -9519,7 +9527,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>166</v>
       </c>
@@ -9554,7 +9562,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>319</v>
       </c>
@@ -9589,7 +9597,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>267</v>
       </c>
@@ -9624,7 +9632,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>88</v>
       </c>
@@ -9659,7 +9667,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>270</v>
       </c>
@@ -9694,7 +9702,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>181</v>
       </c>
@@ -9729,7 +9737,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>185</v>
       </c>
@@ -9764,7 +9772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>183</v>
       </c>
@@ -9799,7 +9807,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -9834,7 +9842,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>204</v>
       </c>
@@ -9869,7 +9877,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>200</v>
       </c>
@@ -9904,7 +9912,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>274</v>
       </c>
@@ -9939,7 +9947,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>276</v>
       </c>
@@ -9974,7 +9982,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>197</v>
       </c>
@@ -10009,7 +10017,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>185</v>
       </c>
@@ -10044,7 +10052,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>199</v>
       </c>
@@ -10079,7 +10087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>321</v>
       </c>
@@ -10114,7 +10122,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>212</v>
       </c>
@@ -10149,7 +10157,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>324</v>
       </c>
@@ -10184,7 +10192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>326</v>
       </c>
@@ -10219,7 +10227,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>181</v>
       </c>
@@ -10254,7 +10262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>327</v>
       </c>
@@ -10289,7 +10297,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>215</v>
       </c>
@@ -10324,7 +10332,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
@@ -10359,7 +10367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>279</v>
       </c>
@@ -10394,7 +10402,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>217</v>
       </c>
@@ -10429,7 +10437,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>329</v>
       </c>
@@ -10464,7 +10472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>188</v>
       </c>
@@ -10499,7 +10507,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>142</v>
       </c>
@@ -10534,7 +10542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>332</v>
       </c>
@@ -10569,7 +10577,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Add overall_end values for stanford 2030
</commit_message>
<xml_diff>
--- a/data/datasets/roster_stanford.xlsx
+++ b/data/datasets/roster_stanford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81139E1-BC24-496E-8482-C7F84A4B542C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D56F7B-1A1B-490C-AD38-82821AF80B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11135,8 +11135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11227,7 +11227,9 @@
       <c r="K2" s="2">
         <v>87</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -11263,7 +11265,9 @@
       <c r="K3" s="2">
         <v>82</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -11299,7 +11303,9 @@
       <c r="K4" s="2">
         <v>77</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -11335,7 +11341,9 @@
       <c r="K5" s="2">
         <v>75</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -11371,7 +11379,9 @@
       <c r="K6" s="2">
         <v>90</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -11407,7 +11417,9 @@
       <c r="K7" s="2">
         <v>87</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -11443,7 +11455,9 @@
       <c r="K8" s="2">
         <v>85</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -11479,7 +11493,9 @@
       <c r="K9" s="2">
         <v>77</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -11515,7 +11531,9 @@
       <c r="K10" s="3">
         <v>73</v>
       </c>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -11551,17 +11569,19 @@
       <c r="K11" s="2">
         <v>84</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>0</v>
@@ -11579,28 +11599,30 @@
         <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>244</v>
+        <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K12" s="2">
-        <v>80</v>
-      </c>
-      <c r="L12" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="L12" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>243</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>239</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>54</v>
@@ -11615,28 +11637,30 @@
         <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>244</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K13" s="2">
-        <v>79</v>
-      </c>
-      <c r="L13" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="L13" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>293</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>294</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>54</v>
@@ -11651,15 +11675,17 @@
         <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K14" s="2">
         <v>79</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -11695,7 +11721,9 @@
       <c r="K15" s="2">
         <v>78</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -11731,7 +11759,9 @@
       <c r="K16" s="2">
         <v>76</v>
       </c>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -11767,7 +11797,9 @@
       <c r="K17" s="2">
         <v>68</v>
       </c>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -11803,7 +11835,9 @@
       <c r="K18" s="2">
         <v>68</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -11839,7 +11873,9 @@
       <c r="K19" s="3">
         <v>66</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3">
+        <v>66</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -11875,7 +11911,9 @@
       <c r="K20" s="2">
         <v>83</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -11911,7 +11949,9 @@
       <c r="K21" s="2">
         <v>74</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -11947,7 +11987,9 @@
       <c r="K22" s="2">
         <v>71</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="2">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -11983,7 +12025,9 @@
       <c r="K23" s="2">
         <v>67</v>
       </c>
-      <c r="L23" s="2"/>
+      <c r="L23" s="2">
+        <v>67</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -12019,7 +12063,9 @@
       <c r="K24" s="2">
         <v>66</v>
       </c>
-      <c r="L24" s="2"/>
+      <c r="L24" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -12055,7 +12101,9 @@
       <c r="K25" s="2">
         <v>65</v>
       </c>
-      <c r="L25" s="2"/>
+      <c r="L25" s="2">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -12091,7 +12139,9 @@
       <c r="K26" s="2">
         <v>83</v>
       </c>
-      <c r="L26" s="2"/>
+      <c r="L26" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -12127,7 +12177,9 @@
       <c r="K27" s="2">
         <v>83</v>
       </c>
-      <c r="L27" s="2"/>
+      <c r="L27" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -12163,7 +12215,9 @@
       <c r="K28" s="2">
         <v>75</v>
       </c>
-      <c r="L28" s="3"/>
+      <c r="L28" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -12199,7 +12253,9 @@
       <c r="K29" s="2">
         <v>75</v>
       </c>
-      <c r="L29" s="2"/>
+      <c r="L29" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -12235,7 +12291,9 @@
       <c r="K30" s="2">
         <v>93</v>
       </c>
-      <c r="L30" s="2"/>
+      <c r="L30" s="2">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -12271,7 +12329,9 @@
       <c r="K31" s="2">
         <v>86</v>
       </c>
-      <c r="L31" s="2"/>
+      <c r="L31" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -12307,7 +12367,9 @@
       <c r="K32" s="2">
         <v>79</v>
       </c>
-      <c r="L32" s="2"/>
+      <c r="L32" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -12343,7 +12405,9 @@
       <c r="K33" s="2">
         <v>68</v>
       </c>
-      <c r="L33" s="2"/>
+      <c r="L33" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -12379,7 +12443,9 @@
       <c r="K34" s="2">
         <v>65</v>
       </c>
-      <c r="L34" s="2"/>
+      <c r="L34" s="2">
+        <v>65</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -12415,7 +12481,9 @@
       <c r="K35" s="2">
         <v>88</v>
       </c>
-      <c r="L35" s="2"/>
+      <c r="L35" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -12451,7 +12519,9 @@
       <c r="K36" s="2">
         <v>81</v>
       </c>
-      <c r="L36" s="2"/>
+      <c r="L36" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -12487,7 +12557,9 @@
       <c r="K37" s="2">
         <v>75</v>
       </c>
-      <c r="L37" s="2"/>
+      <c r="L37" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -12523,7 +12595,9 @@
       <c r="K38" s="2">
         <v>90</v>
       </c>
-      <c r="L38" s="2"/>
+      <c r="L38" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -12559,7 +12633,9 @@
       <c r="K39" s="2">
         <v>78</v>
       </c>
-      <c r="L39" s="2"/>
+      <c r="L39" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -12595,7 +12671,9 @@
       <c r="K40" s="2">
         <v>74</v>
       </c>
-      <c r="L40" s="2"/>
+      <c r="L40" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -12631,7 +12709,9 @@
       <c r="K41" s="2">
         <v>68</v>
       </c>
-      <c r="L41" s="2"/>
+      <c r="L41" s="2">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -12667,7 +12747,9 @@
       <c r="K42" s="2">
         <v>64</v>
       </c>
-      <c r="L42" s="2"/>
+      <c r="L42" s="2">
+        <v>64</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -12703,7 +12785,9 @@
       <c r="K43" s="2">
         <v>88</v>
       </c>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -12739,7 +12823,9 @@
       <c r="K44" s="2">
         <v>86</v>
       </c>
-      <c r="L44" s="2"/>
+      <c r="L44" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -12775,7 +12861,9 @@
       <c r="K45" s="2">
         <v>92</v>
       </c>
-      <c r="L45" s="2"/>
+      <c r="L45" s="2">
+        <v>92</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -12811,7 +12899,9 @@
       <c r="K46" s="2">
         <v>83</v>
       </c>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -12847,7 +12937,9 @@
       <c r="K47" s="2">
         <v>80</v>
       </c>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -12883,7 +12975,9 @@
       <c r="K48" s="2">
         <v>78</v>
       </c>
-      <c r="L48" s="2"/>
+      <c r="L48" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
@@ -12919,7 +13013,9 @@
       <c r="K49" s="2">
         <v>88</v>
       </c>
-      <c r="L49" s="2"/>
+      <c r="L49" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
@@ -12955,7 +13051,9 @@
       <c r="K50" s="2">
         <v>86</v>
       </c>
-      <c r="L50" s="2"/>
+      <c r="L50" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
@@ -12991,7 +13089,9 @@
       <c r="K51" s="2">
         <v>80</v>
       </c>
-      <c r="L51" s="2"/>
+      <c r="L51" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
@@ -13027,7 +13127,9 @@
       <c r="K52" s="2">
         <v>73</v>
       </c>
-      <c r="L52" s="2"/>
+      <c r="L52" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -13063,7 +13165,9 @@
       <c r="K53" s="2">
         <v>73</v>
       </c>
-      <c r="L53" s="2"/>
+      <c r="L53" s="2">
+        <v>73</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
@@ -13099,7 +13203,9 @@
       <c r="K54" s="2">
         <v>90</v>
       </c>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
@@ -13135,7 +13241,9 @@
       <c r="K55" s="2">
         <v>89</v>
       </c>
-      <c r="L55" s="2"/>
+      <c r="L55" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
@@ -13171,7 +13279,9 @@
       <c r="K56" s="2">
         <v>83</v>
       </c>
-      <c r="L56" s="2"/>
+      <c r="L56" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -13207,7 +13317,9 @@
       <c r="K57" s="2">
         <v>76</v>
       </c>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -13243,7 +13355,9 @@
       <c r="K58" s="2">
         <v>71</v>
       </c>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2">
+        <v>71</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
@@ -13279,14 +13393,16 @@
       <c r="K59" s="2">
         <v>88</v>
       </c>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2">
+        <v>90</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -13307,22 +13423,24 @@
         <v>128</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="K60" s="2">
-        <v>75</v>
-      </c>
-      <c r="L60" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="L60" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>25</v>
@@ -13343,15 +13461,17 @@
         <v>128</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="K61" s="2">
-        <v>76</v>
-      </c>
-      <c r="L61" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="L61" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -13387,7 +13507,9 @@
       <c r="K62" s="2">
         <v>86</v>
       </c>
-      <c r="L62" s="2"/>
+      <c r="L62" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
@@ -13423,7 +13545,9 @@
       <c r="K63" s="2">
         <v>84</v>
       </c>
-      <c r="L63" s="2"/>
+      <c r="L63" s="2">
+        <v>85</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -13459,7 +13583,9 @@
       <c r="K64" s="2">
         <v>81</v>
       </c>
-      <c r="L64" s="2"/>
+      <c r="L64" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
@@ -13495,7 +13621,9 @@
       <c r="K65" s="2">
         <v>88</v>
       </c>
-      <c r="L65" s="2"/>
+      <c r="L65" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
@@ -13531,7 +13659,9 @@
       <c r="K66" s="2">
         <v>80</v>
       </c>
-      <c r="L66" s="2"/>
+      <c r="L66" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
@@ -13567,7 +13697,9 @@
       <c r="K67" s="2">
         <v>76</v>
       </c>
-      <c r="L67" s="2"/>
+      <c r="L67" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -13603,17 +13735,19 @@
       <c r="K68" s="2">
         <v>88</v>
       </c>
-      <c r="L68" s="2"/>
+      <c r="L68" s="2">
+        <v>89</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D69" s="1" t="b">
         <v>1</v>
@@ -13631,7 +13765,7 @@
         <v>128</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>22</v>
@@ -13639,17 +13773,19 @@
       <c r="K69" s="2">
         <v>87</v>
       </c>
-      <c r="L69" s="2"/>
+      <c r="L69" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>202</v>
+        <v>276</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>203</v>
+        <v>277</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D70" s="1" t="b">
         <v>1</v>
@@ -13667,7 +13803,7 @@
         <v>128</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>22</v>
@@ -13675,7 +13811,9 @@
       <c r="K70" s="2">
         <v>87</v>
       </c>
-      <c r="L70" s="2"/>
+      <c r="L70" s="2">
+        <v>87</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -13711,7 +13849,9 @@
       <c r="K71" s="2">
         <v>83</v>
       </c>
-      <c r="L71" s="2"/>
+      <c r="L71" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -13747,7 +13887,9 @@
       <c r="K72" s="2">
         <v>83</v>
       </c>
-      <c r="L72" s="2"/>
+      <c r="L72" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
@@ -13783,7 +13925,9 @@
       <c r="K73" s="2">
         <v>83</v>
       </c>
-      <c r="L73" s="2"/>
+      <c r="L73" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
@@ -13819,7 +13963,9 @@
       <c r="K74" s="2">
         <v>77</v>
       </c>
-      <c r="L74" s="2"/>
+      <c r="L74" s="2">
+        <v>77</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
@@ -13855,7 +14001,9 @@
       <c r="K75" s="2">
         <v>86</v>
       </c>
-      <c r="L75" s="2"/>
+      <c r="L75" s="2">
+        <v>88</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
@@ -13891,7 +14039,9 @@
       <c r="K76" s="2">
         <v>83</v>
       </c>
-      <c r="L76" s="2"/>
+      <c r="L76" s="2">
+        <v>83</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -13927,7 +14077,9 @@
       <c r="K77" s="2">
         <v>82</v>
       </c>
-      <c r="L77" s="2"/>
+      <c r="L77" s="2">
+        <v>82</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -13963,7 +14115,9 @@
       <c r="K78" s="2">
         <v>75</v>
       </c>
-      <c r="L78" s="2"/>
+      <c r="L78" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -13999,7 +14153,9 @@
       <c r="K79" s="2">
         <v>67</v>
       </c>
-      <c r="L79" s="2"/>
+      <c r="L79" s="2">
+        <v>67</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
@@ -14035,7 +14191,9 @@
       <c r="K80" s="2">
         <v>80</v>
       </c>
-      <c r="L80" s="2"/>
+      <c r="L80" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
@@ -14071,7 +14229,9 @@
       <c r="K81" s="2">
         <v>74</v>
       </c>
-      <c r="L81" s="2"/>
+      <c r="L81" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -14107,7 +14267,9 @@
       <c r="K82" s="2">
         <v>75</v>
       </c>
-      <c r="L82" s="2"/>
+      <c r="L82" s="2">
+        <v>75</v>
+      </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -14143,7 +14305,9 @@
       <c r="K83" s="2">
         <v>86</v>
       </c>
-      <c r="L83" s="2"/>
+      <c r="L83" s="2">
+        <v>86</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
@@ -14179,7 +14343,9 @@
       <c r="K84" s="2">
         <v>67</v>
       </c>
-      <c r="L84" s="2"/>
+      <c r="L84" s="2">
+        <v>67</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -14215,7 +14381,9 @@
       <c r="K85" s="2">
         <v>78</v>
       </c>
-      <c r="L85" s="2"/>
+      <c r="L85" s="2">
+        <v>78</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
@@ -14251,7 +14419,9 @@
       <c r="K86" s="2">
         <v>66</v>
       </c>
-      <c r="L86" s="2"/>
+      <c r="L86" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>

</xml_diff>